<commit_message>
Fix index reference in the bitstream-metadata sheet
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t xml:space="preserve">BUNDLE-NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROW-ID::1</t>
   </si>
   <si>
     <t xml:space="preserve">import.txt</t>
@@ -369,7 +366,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.41"/>
@@ -537,7 +534,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -556,7 +553,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.82"/>
@@ -588,7 +585,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -607,7 +604,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="92.38"/>
@@ -636,7 +633,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -652,10 +649,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
@@ -683,25 +680,25 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[DSC-721] Bundle creation from bulk import does not set file format
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
@@ -184,7 +184,7 @@
     <t xml:space="preserve">ORIGINAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Test title</t>
+    <t xml:space="preserve">Test title.txt</t>
   </si>
   <si>
     <t xml:space="preserve">test file descr</t>
@@ -366,7 +366,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.41"/>
@@ -534,7 +534,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -553,7 +553,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.82"/>
@@ -585,7 +585,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -604,7 +604,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="92.38"/>
@@ -633,7 +633,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -649,10 +649,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
@@ -698,7 +698,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
DSC-723 BulkImport allows to attach any local files to the items
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
@@ -178,7 +178,7 @@
     <t xml:space="preserve">BUNDLE-NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">import.txt</t>
+    <t xml:space="preserve">THIS IS DYNAMICALLY REPLACED BY THE TEST</t>
   </si>
   <si>
     <t xml:space="preserve">ORIGINAL</t>
@@ -366,7 +366,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.41"/>
@@ -534,7 +534,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -553,7 +553,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.82"/>
@@ -585,7 +585,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -604,7 +604,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="92.38"/>
@@ -633,7 +633,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -649,10 +649,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
@@ -698,7 +698,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[DSC-844] Improve handling of bitstream metadata in BulkImport
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t xml:space="preserve">BUNDLE-NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BITSTREAM-ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCESS-CONDITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDITIONAL-ACCESS-CONDITION</t>
   </si>
   <si>
     <t xml:space="preserve">THIS IS DYNAMICALLY REPLACED BY THE TEST</t>
@@ -270,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,6 +290,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -363,10 +384,10 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.41"/>
@@ -534,7 +555,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -550,10 +571,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.82"/>
@@ -585,7 +606,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -601,10 +622,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="92.38"/>
@@ -633,7 +654,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -646,19 +667,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:F"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,9 +696,18 @@
         <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -683,22 +716,38 @@
         <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>54</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="G2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[DSC-844] Improved bitstreams handling during BulkImport
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
@@ -178,7 +178,7 @@
     <t xml:space="preserve">BUNDLE-NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">BITSTREAM-ID</t>
+    <t xml:space="preserve">POSITION</t>
   </si>
   <si>
     <t xml:space="preserve">ACCESS-CONDITION</t>
@@ -187,7 +187,25 @@
     <t xml:space="preserve">ADDITIONAL-ACCESS-CONDITION</t>
   </si>
   <si>
-    <t xml:space="preserve">THIS IS DYNAMICALLY REPLACED BY THE TEST</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">file://test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.txt</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ORIGINAL</t>
@@ -231,7 +249,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF2A6099"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -313,66 +331,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF2A6099"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -384,10 +342,10 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.41"/>
@@ -571,10 +529,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.82"/>
@@ -622,10 +580,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="92.38"/>
@@ -670,15 +628,15 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:F"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
@@ -745,12 +703,15 @@
       <c r="D6" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="file://test"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>